<commit_message>
Added issues numbers for some waived holes.
Signed-off-by: Pascal Gouedo <pascal.gouedo@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_waiver_list.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_v1.8.0/CV32E40Pv2_waiver_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scorpion\Scorpion\kagao0\LocalStock\bnl\cv32\repo\program\update_cv32e40pv2_rpt_WW23\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\core-v-docs\Project-Descriptions-and-Plans\CV32E40Pv2\Milestone-data\RTL_v1.8.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5490E8BA-2403-488A-BEC9-9C36C85971D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8653A3BB-594A-43F9-82F9-1818841C0638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" summary" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="314">
   <si>
     <t>code cov waiver</t>
   </si>
@@ -973,6 +973,19 @@
   </si>
   <si>
     <t>feccondrow 1241 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv32e40p issue no. </t>
+  </si>
+  <si>
+    <t>#1004</t>
+  </si>
+  <si>
+    <t>#1005</t>
+  </si>
+  <si>
+    <t>#1006
+#1007</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1601,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1653,6 +1666,10 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2079,7 +2096,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A3:D75" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="A3:D75" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="core-v-verif issue no. "/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="cv32e40p issue no. "/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category S/N"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reason" dataDxfId="60"/>
     <tableColumn id="4" xr3:uid="{DD5C4403-AE4E-4AEB-8C14-4110540FE3EE}" name="configuration applicable for waiver"/>
@@ -2526,7 +2543,7 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2548,7 +2565,7 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>310</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>129</v>
@@ -2840,6 +2857,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
       <c r="B31">
         <v>28</v>
       </c>
@@ -2851,6 +2869,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
       <c r="B32">
         <v>29</v>
       </c>
@@ -2862,8 +2881,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>281</v>
+      <c r="A33" s="25" t="s">
+        <v>311</v>
       </c>
       <c r="B33">
         <v>30</v>
@@ -2876,8 +2895,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>281</v>
+      <c r="A34" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="B34">
         <v>31</v>
@@ -2890,8 +2909,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
-        <v>281</v>
+      <c r="A35" s="26" t="s">
+        <v>313</v>
       </c>
       <c r="B35">
         <v>32</v>
@@ -2904,6 +2923,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="25"/>
       <c r="B36">
         <v>33</v>
       </c>
@@ -2915,6 +2935,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
       <c r="B37">
         <v>34</v>
       </c>
@@ -2926,6 +2947,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="25"/>
       <c r="B38">
         <v>35</v>
       </c>
@@ -2937,6 +2959,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="25"/>
       <c r="B39">
         <v>36</v>
       </c>
@@ -2948,6 +2971,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="25"/>
       <c r="B40">
         <v>37</v>
       </c>
@@ -3421,6 +3445,7 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A78:D78"/>
   </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
@@ -19840,6 +19865,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
@@ -19848,15 +19882,6 @@
     <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20109,6 +20134,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D755283-77AF-467A-8C74-DC8595DDCA72}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
@@ -20121,14 +20154,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>